<commit_message>
Répartition Heures : Ajout developper 2 : Loan Lassalle
</commit_message>
<xml_diff>
--- a/Administratif/Répartition_heures.xlsx
+++ b/Administratif/Répartition_heures.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18708" windowHeight="8736"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18705" windowHeight="8730"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -439,6 +439,135 @@
         </r>
       </text>
     </comment>
+    <comment ref="D6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Analyse du projet
+Mise en place
+Rapport</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Création de la base de données
+Rapport</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Code de liaison entre la base de données et le programme Java
+Intégration au projet
+Tests
+Rapport</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Intégration au projet
+Ajout des fonctionnalité supplémentaires
+Correction des problèmes
+Rapport</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Auteur:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Présentation</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -455,9 +584,6 @@
     <t>33h / 6 = 5.5h de travail par semaine et par développeur</t>
   </si>
   <si>
-    <t>Développeur 2</t>
-  </si>
-  <si>
     <t>Développeur 3</t>
   </si>
   <si>
@@ -549,13 +675,16 @@
   </si>
   <si>
     <t>Groupe JE sais pas</t>
+  </si>
+  <si>
+    <t>Loan Lassalle</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -585,6 +714,13 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
@@ -976,89 +1112,89 @@
   <dimension ref="A1:R21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+      <selection activeCell="AE18" sqref="AE18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.109375" style="7" customWidth="1"/>
-    <col min="2" max="17" width="5.33203125" style="2" customWidth="1"/>
-    <col min="18" max="18" width="8.77734375" style="10" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" style="7" customWidth="1"/>
+    <col min="2" max="17" width="5.28515625" style="2" customWidth="1"/>
+    <col min="18" max="18" width="8.7109375" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
       <c r="D1" s="11"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
       <c r="D2" s="11"/>
     </row>
-    <row r="4" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
       <c r="B4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="F4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="G4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="H4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="I4" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="J4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="K4" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="L4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="L4" s="4" t="s">
+      <c r="M4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="M4" s="4" t="s">
+      <c r="N4" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="N4" s="4" t="s">
+      <c r="O4" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="O4" s="4" t="s">
+      <c r="P4" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="P4" s="4" t="s">
+      <c r="Q4" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="Q4" s="4" t="s">
+      <c r="R4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="R4" s="4" t="s">
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>33</v>
       </c>
       <c r="B5" s="1">
         <v>2.5</v>
@@ -1113,36 +1249,66 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="1">
         <v>3</v>
       </c>
-      <c r="B6" s="1">
+      <c r="C6" s="1">
+        <v>3</v>
+      </c>
+      <c r="D6" s="1">
+        <v>5.5</v>
+      </c>
+      <c r="E6" s="1">
+        <v>6</v>
+      </c>
+      <c r="F6" s="1">
+        <v>6</v>
+      </c>
+      <c r="G6" s="1">
+        <v>6</v>
+      </c>
+      <c r="H6" s="1">
+        <v>7</v>
+      </c>
+      <c r="I6" s="1">
+        <v>7</v>
+      </c>
+      <c r="J6" s="1">
+        <v>7</v>
+      </c>
+      <c r="K6" s="1">
+        <v>7</v>
+      </c>
+      <c r="L6" s="1">
+        <v>5.5</v>
+      </c>
+      <c r="M6" s="1">
+        <v>5.5</v>
+      </c>
+      <c r="N6" s="1">
+        <v>5.5</v>
+      </c>
+      <c r="O6" s="1">
+        <v>5.5</v>
+      </c>
+      <c r="P6" s="1">
+        <v>5.5</v>
+      </c>
+      <c r="Q6" s="1">
         <v>5</v>
       </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
-      <c r="Q6" s="1"/>
       <c r="R6" s="4">
         <f t="shared" ref="R6:R10" si="0">SUM(B6:Q6)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7" s="1">
         <v>6</v>
@@ -1167,9 +1333,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" s="1">
         <v>5</v>
@@ -1194,9 +1360,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" s="1">
         <v>6</v>
@@ -1221,9 +1387,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" s="1">
         <v>6</v>
@@ -1248,129 +1414,129 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B11" s="4">
         <f>SUM(B5:B10)</f>
-        <v>30.5</v>
+        <v>28.5</v>
       </c>
       <c r="C11" s="4">
         <f t="shared" ref="C11:Q11" si="1">SUM(C5:C10)</f>
-        <v>5.5</v>
+        <v>8.5</v>
       </c>
       <c r="D11" s="4">
         <f t="shared" si="1"/>
-        <v>5.5</v>
+        <v>11</v>
       </c>
       <c r="E11" s="4">
         <f t="shared" si="1"/>
-        <v>6.5</v>
+        <v>12.5</v>
       </c>
       <c r="F11" s="4">
         <f t="shared" si="1"/>
-        <v>5.5</v>
+        <v>11.5</v>
       </c>
       <c r="G11" s="4">
         <f t="shared" si="1"/>
-        <v>5.5</v>
+        <v>11.5</v>
       </c>
       <c r="H11" s="4">
         <f t="shared" si="1"/>
-        <v>5.5</v>
+        <v>12.5</v>
       </c>
       <c r="I11" s="4">
         <f t="shared" si="1"/>
-        <v>5.5</v>
+        <v>12.5</v>
       </c>
       <c r="J11" s="4">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="K11" s="4">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="L11" s="4">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>12.5</v>
       </c>
       <c r="M11" s="4">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>13.5</v>
       </c>
       <c r="N11" s="4">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>13.5</v>
       </c>
       <c r="O11" s="4">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>10.5</v>
       </c>
       <c r="P11" s="4">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>10.5</v>
       </c>
       <c r="Q11" s="4">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="R11" s="12">
         <f>SUM(R5:R10)</f>
-        <v>118</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B13" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A14" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B15" s="8" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B16" s="8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="8" t="s">
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B20" s="8" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="8" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B21" s="8" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Répartiton heures : developpeur 2 Loan Lassalle correction merged
</commit_message>
<xml_diff>
--- a/Administratif/Répartition_heures.xlsx
+++ b/Administratif/Répartition_heures.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Utilisateurs\Lassalle Loan\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Utilisateurs\Lassalle Loan\Cloud Station\Documents\Etudes\HEIG\2ième Année Bachelor (2016-2017)\2ième Semestre\PRO\projetHeig\Administratif\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -557,7 +557,7 @@
           </rPr>
           <t xml:space="preserve">
 Intégration au projet
-Ajout des fonctionnalité supplémentaires
+Ajout des fonctionnalités supplémentaires
 Correction des problèmes
 Rapport</t>
         </r>
@@ -3814,7 +3814,7 @@
   <dimension ref="A1:R21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R20" sqref="R20"/>
+      <selection activeCell="X10" sqref="X10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Répartiton heures : correction merged_2
</commit_message>
<xml_diff>
--- a/Administratif/Répartition_heures.xlsx
+++ b/Administratif/Répartition_heures.xlsx
@@ -27,6 +27,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author/>
+    <author>Lassalle Loan</author>
     <author>Auteur</author>
   </authors>
   <commentList>
@@ -458,7 +459,31 @@
         </r>
       </text>
     </comment>
-    <comment ref="D6" authorId="1" shapeId="0">
+    <comment ref="B6" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Lassalle Loan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Recherche de sujets</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D6" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -484,7 +509,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E6" authorId="1" shapeId="0">
+    <comment ref="E6" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -509,7 +534,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H6" authorId="1" shapeId="0">
+    <comment ref="H6" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -536,7 +561,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L6" authorId="1" shapeId="0">
+    <comment ref="L6" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -563,7 +588,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P6" authorId="1" shapeId="0">
+    <comment ref="P6" authorId="2" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -3814,7 +3839,7 @@
   <dimension ref="A1:R21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X10" sqref="X10"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
camilo repartitions heures vDone
</commit_message>
<xml_diff>
--- a/Administratif/Répartition_heures.xlsx
+++ b/Administratif/Répartition_heures.xlsx
@@ -29,6 +29,7 @@
     <author/>
     <author>Lassalle Loan</author>
     <author>Auteur</author>
+    <author>camilo</author>
   </authors>
   <commentList>
     <comment ref="B5" authorId="0" shapeId="0">
@@ -609,6 +610,401 @@
           </rPr>
           <t xml:space="preserve">
 Présentation</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B8" authorId="3" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>camilo:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+mise en place groupes, mise en place workspace git, discussuion sujet et choix gestionnaire mdp</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C8" authorId="3" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>camilo:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+recherche second sujet
+sessions de crise</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D8" authorId="3" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>camilo:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+cahier des charges</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E8" authorId="3" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>camilo:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+4 fct. Pdf et génération de fichiers</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F8" authorId="3" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>camilo:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+pdf 2h
+base de donnée 4h</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G8" authorId="3" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>camilo:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+base de donnée 2h
+GUI 4h</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H8" authorId="3" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>camilo:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+rapport 3h
+pdf 3h</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I8" authorId="3" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>camilo:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+GUI 4h
+documentation 2h</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J8" authorId="3" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>camilo:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+tests pdf 3h
+GUI 3h</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K8" authorId="3" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>camilo:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+mise en cummun 3h
+documentation 3h</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L8" authorId="3" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>camilo:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+documentation
+rapport 3h
+mise en commun 3h</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M8" authorId="3" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>camilo:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+tests 3h
+debug 3h</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N8" authorId="3" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>camilo:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+rapport et documentation 4h
+tests 2h</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O8" authorId="3" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>camilo:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+mise en forme rapport et documentation</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P8" authorId="3" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>camilo:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+préparation présentation</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q8" authorId="3" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>camilo:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+présentation, répétition, présentation</t>
         </r>
       </text>
     </comment>
@@ -1359,7 +1755,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1411,6 +1807,27 @@
       <name val="Tahoma"/>
       <charset val="1"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1453,7 +1870,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1485,6 +1902,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -4161,7 +4581,7 @@
   <dimension ref="A1:R21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4415,26 +4835,56 @@
         <v>34</v>
       </c>
       <c r="B8" s="10">
-        <v>5</v>
-      </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
-      <c r="N8" s="10"/>
-      <c r="O8" s="10"/>
-      <c r="P8" s="10"/>
-      <c r="Q8" s="10"/>
+        <v>4</v>
+      </c>
+      <c r="C8" s="15">
+        <v>6</v>
+      </c>
+      <c r="D8" s="10">
+        <v>4</v>
+      </c>
+      <c r="E8" s="10">
+        <v>4</v>
+      </c>
+      <c r="F8" s="10">
+        <v>6</v>
+      </c>
+      <c r="G8" s="10">
+        <v>6</v>
+      </c>
+      <c r="H8" s="10">
+        <v>6</v>
+      </c>
+      <c r="I8" s="10">
+        <v>6</v>
+      </c>
+      <c r="J8" s="10">
+        <v>6</v>
+      </c>
+      <c r="K8" s="10">
+        <v>6</v>
+      </c>
+      <c r="L8" s="10">
+        <v>6</v>
+      </c>
+      <c r="M8" s="10">
+        <v>6</v>
+      </c>
+      <c r="N8" s="10">
+        <v>6</v>
+      </c>
+      <c r="O8" s="10">
+        <v>6</v>
+      </c>
+      <c r="P8" s="10">
+        <v>6</v>
+      </c>
+      <c r="Q8" s="10">
+        <v>6</v>
+      </c>
       <c r="R8" s="7">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
@@ -4557,71 +5007,71 @@
       </c>
       <c r="B11" s="7">
         <f t="shared" ref="B11:R11" si="2">SUM(B5:B10)</f>
-        <v>23.5</v>
+        <v>22.5</v>
       </c>
       <c r="C11" s="7">
         <f t="shared" si="2"/>
-        <v>19.5</v>
+        <v>25.5</v>
       </c>
       <c r="D11" s="7">
         <f t="shared" si="2"/>
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E11" s="7">
         <f t="shared" si="2"/>
-        <v>23.5</v>
+        <v>27.5</v>
       </c>
       <c r="F11" s="7">
         <f t="shared" si="2"/>
-        <v>21.5</v>
+        <v>27.5</v>
       </c>
       <c r="G11" s="7">
         <f t="shared" si="2"/>
-        <v>22.5</v>
+        <v>28.5</v>
       </c>
       <c r="H11" s="7">
         <f t="shared" si="2"/>
-        <v>23.5</v>
+        <v>29.5</v>
       </c>
       <c r="I11" s="7">
         <f t="shared" si="2"/>
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="J11" s="7">
         <f t="shared" si="2"/>
-        <v>25.5</v>
+        <v>31.5</v>
       </c>
       <c r="K11" s="7">
         <f t="shared" si="2"/>
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="L11" s="7">
         <f t="shared" si="2"/>
-        <v>25.5</v>
+        <v>31.5</v>
       </c>
       <c r="M11" s="7">
         <f t="shared" si="2"/>
-        <v>26.5</v>
+        <v>32.5</v>
       </c>
       <c r="N11" s="7">
         <f t="shared" si="2"/>
-        <v>26.5</v>
+        <v>32.5</v>
       </c>
       <c r="O11" s="7">
         <f t="shared" si="2"/>
-        <v>20.5</v>
+        <v>26.5</v>
       </c>
       <c r="P11" s="7">
         <f t="shared" si="2"/>
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="Q11" s="7">
         <f t="shared" si="2"/>
-        <v>19.5</v>
+        <v>25.5</v>
       </c>
       <c r="R11" s="11">
         <f t="shared" si="2"/>
-        <v>370</v>
+        <v>455</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
@@ -4688,8 +5138,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>